<commit_message>
Transformer design is going on.
</commit_message>
<xml_diff>
--- a/Transformer Design.xlsx
+++ b/Transformer Design.xlsx
@@ -19,47 +19,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Design Inputs</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>Temp Min</t>
-  </si>
-  <si>
-    <t>Temp Max</t>
-  </si>
-  <si>
     <t>Initial Calculations</t>
   </si>
   <si>
     <t>N1/N2</t>
   </si>
   <si>
-    <t>CurrIn</t>
-  </si>
-  <si>
-    <t>CurrOut</t>
-  </si>
-  <si>
-    <t>Vin</t>
-  </si>
-  <si>
-    <t>Vo</t>
-  </si>
-  <si>
     <t>Core Specs</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Core Dependent Calculations</t>
   </si>
   <si>
@@ -69,17 +42,133 @@
     <t>N2</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Edge</t>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>CoreLoss(W/kg)</t>
+  </si>
+  <si>
+    <t>Density(kg/dm3)</t>
+  </si>
+  <si>
+    <t>J(A/mm2)</t>
+  </si>
+  <si>
+    <t>Window Area(m2)</t>
+  </si>
+  <si>
+    <t>Window Edge(m)</t>
+  </si>
+  <si>
+    <t>S(VA)</t>
+  </si>
+  <si>
+    <t>Vin(Vrms)</t>
+  </si>
+  <si>
+    <t>Vo(Vrms)</t>
+  </si>
+  <si>
+    <t>f(Hz)</t>
+  </si>
+  <si>
+    <t>Temp Min(Celc)</t>
+  </si>
+  <si>
+    <t>Temp Max(Celc)</t>
+  </si>
+  <si>
+    <t>B(T)</t>
+  </si>
+  <si>
+    <t>Relative Perm</t>
+  </si>
+  <si>
+    <t>Lamination Thickness(m)</t>
+  </si>
+  <si>
+    <t>CurrIn(Arms)</t>
+  </si>
+  <si>
+    <t>CurrOut(Arms)</t>
+  </si>
+  <si>
+    <t>AreaCopperIn(m2)</t>
+  </si>
+  <si>
+    <t>AreaCopperOut(m2)</t>
+  </si>
+  <si>
+    <t>Area(m2)</t>
+  </si>
+  <si>
+    <t>H(A/m)</t>
+  </si>
+  <si>
+    <t>OuterEdge(m)</t>
+  </si>
+  <si>
+    <t>Middle Length(m)</t>
+  </si>
+  <si>
+    <t>Winding Specs</t>
+  </si>
+  <si>
+    <t>One Turn Length(m)</t>
+  </si>
+  <si>
+    <t>Resistivity(ohm-m) @20C</t>
+  </si>
+  <si>
+    <t>Temperature Coeff</t>
+  </si>
+  <si>
+    <t>Winding Calculations</t>
+  </si>
+  <si>
+    <t>Input Wind. Resist @50C</t>
+  </si>
+  <si>
+    <t>Output Wind. Resist @50C</t>
+  </si>
+  <si>
+    <t>Copper Mass(kg)</t>
+  </si>
+  <si>
+    <t>Density(kg/m3)</t>
+  </si>
+  <si>
+    <t>Edge(m)</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Core Mass(kg)</t>
+  </si>
+  <si>
+    <t>Efficiency(%)</t>
+  </si>
+  <si>
+    <t>Copper Loss(W)</t>
+  </si>
+  <si>
+    <t>Core Loss(W)</t>
+  </si>
+  <si>
+    <t>Total Loss(W)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +194,31 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +229,21 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
@@ -138,24 +265,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="İyi" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Virgül" xfId="1" builtinId="3"/>
+    <cellStyle name="Vurgu1" xfId="3" builtinId="29"/>
+    <cellStyle name="Vurgu5" xfId="4" builtinId="45"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,157 +576,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>500000</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <f>B3/B4</f>
         <v>1.38</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="13">
+        <f>E3*E3*E20+E4*E4*E21</f>
+        <v>1984.450525028923</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2">
         <v>34500</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6">
         <f>B2/B3</f>
         <v>14.492753623188406</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="15">
+        <f>B14*E18</f>
+        <v>2078.3955122937696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>25000</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <f>B2/B4</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H2+H3</f>
+        <v>4062.8460373226926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <f>E2*B10</f>
+        <v>1793.9999999999998</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="16">
+        <f>100*B2/(B2+H4)</f>
+        <v>99.193980260742748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>-30</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6">
+        <f>E5*(E3*SQRT(2)/B9*0.000001)</f>
+        <v>1.2256517540566824E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6">
+        <f>B10*(E4*SQRT(2)/B9*0.000001)</f>
+        <v>1.2256517540566824E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="6">
+        <f>(E6+E7)/B8</f>
+        <v>8.1710116937112165E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="6">
+        <f>SQRT(E8)</f>
+        <v>0.28584981535259413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="5">
-        <f>E2*B11</f>
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="5">
-        <f>B3/(B5*E10*B10)</f>
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.5</v>
+      </c>
       <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7">
-        <f>SQRT(E11)</f>
-        <v>0.6454972243679028</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="E12" s="4">
+        <f>B3/(4.44*B5*E5*B12)</f>
+        <v>5.7750057750057752E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <v>610</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="6">
+        <f>SQRT(E12)</f>
+        <v>0.24031241697019684</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="10">
+        <f>B12/(B13*4*0.0000001*PI())</f>
+        <v>1956.8230708019921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5">
+        <v>3.5E-4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="9">
+        <f>E13*2+E9</f>
+        <v>0.76647464929298781</v>
+      </c>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="6">
+        <f>(E9+E13)*4</f>
+        <v>2.1046489292911641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="9">
+        <f>4*E13</f>
+        <v>0.96124966788078736</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="4">
+        <f>E12*E16*B16*1000</f>
+        <v>923.73133879723082</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2">
+        <v>8940</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="4">
+        <f>(B21*(B7-20)*B22 + B21)*E5*E17/(E6/E5)</f>
+        <v>4.7239844748313509</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1.6800000000000002E-8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="4">
+        <f>(B21*(B7-20)*B22 + B21)*B10*E17/(E7/B10)</f>
+        <v>2.4805631562861539</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3.8E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="11">
+        <f>(B20*E6*E17)+(B20*E7*B10)</f>
+        <v>142550.57412279991</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Transformer Design is completed. Report will be started.
</commit_message>
<xml_diff>
--- a/Transformer Design.xlsx
+++ b/Transformer Design.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Design Inputs</t>
   </si>
@@ -93,12 +93,6 @@
     <t>CurrOut(Arms)</t>
   </si>
   <si>
-    <t>AreaCopperIn(m2)</t>
-  </si>
-  <si>
-    <t>AreaCopperOut(m2)</t>
-  </si>
-  <si>
     <t>Area(m2)</t>
   </si>
   <si>
@@ -157,18 +151,59 @@
   </si>
   <si>
     <t>Total Loss(W)</t>
+  </si>
+  <si>
+    <t>N2*AreaCopperOut(mm2)</t>
+  </si>
+  <si>
+    <t>N1*AreaCopperIn(mm2)</t>
+  </si>
+  <si>
+    <t>Inductance Calculations</t>
+  </si>
+  <si>
+    <t>Reluctance</t>
+  </si>
+  <si>
+    <t>Mutual Inductance(H)</t>
+  </si>
+  <si>
+    <t>Leakage Ind 1 (H)</t>
+  </si>
+  <si>
+    <t>Leakage Ind 2 (H)</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Material Cost</t>
+  </si>
+  <si>
+    <t>Core Cost ($/kg)</t>
+  </si>
+  <si>
+    <t>Winding Cost ($/kg)</t>
+  </si>
+  <si>
+    <t>Energy Lost (0.07$/kwh)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="8">
+    <numFmt numFmtId="44" formatCode="_-&quot;₺&quot;* #,##0.00_-;\-&quot;₺&quot;* #,##0.00_-;_-&quot;₺&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;_ ;_-@_ "/>
+    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0_ ;_-[$$-409]* \-#,##0\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,8 +252,16 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +289,11 @@
         <fgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -265,37 +313,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="6" fillId="6" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="6" fillId="6" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="5" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="İyi" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nötr" xfId="6" builtinId="28"/>
+    <cellStyle name="ParaBirimi" xfId="5" builtinId="4"/>
     <cellStyle name="Virgül" xfId="1" builtinId="3"/>
     <cellStyle name="Vurgu1" xfId="3" builtinId="29"/>
     <cellStyle name="Vurgu5" xfId="4" builtinId="45"/>
@@ -576,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,25 +646,25 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="G1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="8"/>
+      <c r="E1" s="23"/>
+      <c r="G1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -617,16 +676,16 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="11">
         <f>B3/B4</f>
         <v>1.38</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="13">
-        <f>E3*E3*E20+E4*E4*E21</f>
-        <v>1984.450525028923</v>
+        <v>41</v>
+      </c>
+      <c r="H2" s="7">
+        <f>E3*E3*E21+E4*E4*E22</f>
+        <v>1173.6473261855806</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -639,16 +698,16 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="11">
         <f>B2/B3</f>
         <v>14.492753623188406</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="15">
+        <v>42</v>
+      </c>
+      <c r="H3" s="8">
         <f>B14*E18</f>
-        <v>2078.3955122937696</v>
+        <v>11536.365774997474</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,16 +720,16 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <f>B2/B4</f>
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="12">
+        <v>43</v>
+      </c>
+      <c r="H4" s="6">
         <f>H2+H3</f>
-        <v>4062.8460373226926</v>
+        <v>12710.013101183054</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -683,16 +742,16 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="17">
         <f>E2*B10</f>
-        <v>1793.9999999999998</v>
+        <v>345</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="16">
+        <v>40</v>
+      </c>
+      <c r="H5" s="9">
         <f>100*B2/(B2+H4)</f>
-        <v>99.193980260742748</v>
+        <v>97.521013286964077</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,11 +762,11 @@
         <v>-30</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6">
-        <f>E5*(E3*SQRT(2)/B9*0.000001)</f>
-        <v>1.2256517540566824E-2</v>
+        <v>45</v>
+      </c>
+      <c r="E6" s="11">
+        <f>E5*(E3/B9)</f>
+        <v>1666.6666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -718,11 +777,11 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="6">
-        <f>B10*(E4*SQRT(2)/B9*0.000001)</f>
-        <v>1.2256517540566824E-2</v>
+        <v>44</v>
+      </c>
+      <c r="E7" s="11">
+        <f>B10*(E4/B9)</f>
+        <v>1666.6666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -735,9 +794,9 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="6">
-        <f>(E6+E7)/B8</f>
-        <v>8.1710116937112165E-2</v>
+      <c r="E8" s="13">
+        <f>(E6+E7)*0.000001/B8</f>
+        <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,42 +809,53 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="14">
         <f>SQRT(E8)</f>
-        <v>0.28584981535259413</v>
+        <v>0.10540925533894598</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5">
-        <v>1300</v>
+      <c r="B10" s="21">
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="D11" s="8" t="s">
+      <c r="B11" s="23"/>
+      <c r="D11" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="23"/>
+      <c r="G11" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="3">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="4">
+        <v>24</v>
+      </c>
+      <c r="E12" s="10">
         <f>B3/(4.44*B5*E5*B12)</f>
-        <v>5.7750057750057752E-2</v>
+        <v>0.3753753753753753</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="22">
+        <f>E16/(E12*B13*4*PI()*0.0000001)</f>
+        <v>12846.468022061199</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -793,14 +863,21 @@
         <v>20</v>
       </c>
       <c r="B13" s="2">
-        <v>610</v>
+        <v>474</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="6">
+        <v>37</v>
+      </c>
+      <c r="E13" s="11">
         <f>SQRT(E12)</f>
-        <v>0.24031241697019684</v>
+        <v>0.61267885174483971</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="16">
+        <f>E5*E5/H12</f>
+        <v>9.2651925646487996</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,131 +885,177 @@
         <v>8</v>
       </c>
       <c r="B14" s="2">
-        <v>2.25</v>
+        <v>1.363</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="10">
+        <v>25</v>
+      </c>
+      <c r="E14" s="12">
         <f>B12/(B13*4*0.0000001*PI())</f>
-        <v>1956.8230708019921</v>
+        <v>2014.6195328088015</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="15">
+        <f>(B3/E3)*0.02/(2*PI()*B5)</f>
+        <v>0.15154733681210272</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>3.5E-4</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="9">
+        <v>26</v>
+      </c>
+      <c r="E15" s="15">
         <f>E13*2+E9</f>
-        <v>0.76647464929298781</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>1.3307669588286255</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="15">
+        <f>(B4/E4)*0.02/(2*PI()*B5)</f>
+        <v>7.9577471545947673E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="2">
-        <v>7.6</v>
+        <v>7.85</v>
       </c>
       <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="11">
+        <f>(E9+E13)*4</f>
+        <v>2.8723524283351427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="6">
-        <f>(E9+E13)*4</f>
-        <v>2.1046489292911641</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="D17" t="s">
+      <c r="E17" s="15">
+        <f>(E9/2+E13)*PI()</f>
+        <v>2.0903638507480204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="18">
+        <f>E12*E16*B16*1000</f>
+        <v>8463.9514123238987</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="D20" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="G20" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8940</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="11">
+        <f>(B22*(B7-20)*B23 + B22)*E5*E17/(E6*0.000001/E5)</f>
+        <v>2.7938674599847748</v>
+      </c>
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="19">
+        <f>E23*B24 + E18*B17</f>
+        <v>25890.196978990025</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1.6800000000000002E-8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="11">
+        <f>(B22*(B7-20)*B23 + B22)*B10*E17/(E7*0.000001/B10)</f>
+        <v>1.4670591577319758</v>
+      </c>
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="20">
+        <f>(H4/1000)*20*365*24*0.07</f>
+        <v>155875.600672909</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="9">
-        <f>4*E13</f>
-        <v>0.96124966788078736</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="4">
-        <f>E12*E16*B16*1000</f>
-        <v>923.73133879723082</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="D19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="2">
-        <v>8940</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B23" s="2">
+        <v>3.8E-3</v>
+      </c>
+      <c r="D23" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="4">
-        <f>(B21*(B7-20)*B22 + B21)*E5*E17/(E6/E5)</f>
-        <v>4.7239844748313509</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1.6800000000000002E-8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="4">
-        <f>(B21*(B7-20)*B22 + B21)*B10*E17/(E7/B10)</f>
-        <v>2.4805631562861539</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2">
-        <v>3.8E-3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="11">
-        <f>(B20*E6*E17)+(B20*E7*B10)</f>
-        <v>142550.57412279991</v>
+      <c r="E23" s="17">
+        <f>(B21*E6*0.000001*E17)+(B21*E7*0.000001*E17)</f>
+        <v>62.292842752291001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>